<commit_message>
trying to calcualte PiN with EMMM
</commit_message>
<xml_diff>
--- a/input/Template_EMIS_Access.xlsx
+++ b/input/Template_EMIS_Access.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="433" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{765B3A74-2B1B-404D-908F-38838E10F202}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
+    <workbookView xWindow="-19290" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
   </bookViews>
   <sheets>
     <sheet name="indicator" sheetId="3" r:id="rId1"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>